<commit_message>
Changes in response to reviews
</commit_message>
<xml_diff>
--- a/Setting/inputs/Setting.xlsx
+++ b/Setting/inputs/Setting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/Setting/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFBECB3-566D-5D46-8F29-BEF236283ED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70C2D0A4-77B3-B644-AAB4-111314A290D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="1780" windowWidth="20420" windowHeight="9860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="2540" windowWidth="20420" windowHeight="9860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="291">
   <si>
     <t>BCIO_ID</t>
   </si>
@@ -1672,6 +1672,9 @@
   </si>
   <si>
     <t>geographic location [GAZ:00000448]</t>
+  </si>
+  <si>
+    <t>BCIO:026051</t>
   </si>
 </sst>
 </file>
@@ -2096,8 +2099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3048,7 +3051,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>84</v>
+        <v>290</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>242</v>
@@ -4225,6 +4228,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC046B428994B048B5D1607E2BC0A9EE" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39e35c52df37ff2180535b714fdb036d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fa734e6e-2dd8-4275-9b08-04e206339f53" xmlns:ns3="ac97e7bc-1267-463a-8e0a-d8030d117d70" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="93c719530b81246d128a373b780dc003" ns2:_="" ns3:_="">
     <xsd:import namespace="fa734e6e-2dd8-4275-9b08-04e206339f53"/>
@@ -4441,22 +4459,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF9454A1-A395-40F6-B8A5-B468B9176A79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F469C38F-E02B-4811-BC50-AB2CCD2039A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D1C1A7-69A1-4E05-8965-878EE9650465}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4473,21 +4493,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F469C38F-E02B-4811-BC50-AB2CCD2039A2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF9454A1-A395-40F6-B8A5-B468B9176A79}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change ID column name  for template
</commit_message>
<xml_diff>
--- a/Setting/inputs/Setting.xlsx
+++ b/Setting/inputs/Setting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/Setting/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548299E9-1B4D-8B4A-BDFA-6BE46CA3838F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D176A661-8CFA-7848-9F0D-547F53A89237}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2100" yWindow="2540" windowWidth="20420" windowHeight="9860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="297">
   <si>
-    <t>BCIO_ID</t>
-  </si>
-  <si>
     <t>Definition</t>
   </si>
   <si>
@@ -1693,6 +1690,9 @@
   </si>
   <si>
     <t>Discussed</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -2117,8 +2117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M62" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2136,81 +2136,81 @@
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="6" t="s">
-        <v>4</v>
-      </c>
       <c r="R1" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="T1" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="S1" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>294</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="8"/>
@@ -2222,30 +2222,30 @@
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="T2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="8"/>
@@ -2257,28 +2257,28 @@
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="T3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="8"/>
@@ -2290,31 +2290,31 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
       <c r="P4" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="T4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -2325,7 +2325,7 @@
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
@@ -2333,18 +2333,18 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="T5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -2355,28 +2355,28 @@
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
       <c r="T6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="8"/>
@@ -2388,28 +2388,28 @@
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
       <c r="T7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="8"/>
@@ -2421,28 +2421,28 @@
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
       <c r="T8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -2453,7 +2453,7 @@
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
@@ -2461,18 +2461,18 @@
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="T9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="8"/>
@@ -2484,30 +2484,30 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
       <c r="T10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="8"/>
@@ -2519,7 +2519,7 @@
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -2527,18 +2527,18 @@
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
       <c r="T11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="8"/>
@@ -2550,30 +2550,30 @@
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
       <c r="T12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="8"/>
@@ -2585,30 +2585,30 @@
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O13" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="N13" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="O13" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
       <c r="T13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="8"/>
@@ -2620,30 +2620,30 @@
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O14" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="T14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="8"/>
@@ -2655,30 +2655,30 @@
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="N15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="O15" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="T15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="8"/>
@@ -2690,7 +2690,7 @@
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
@@ -2698,18 +2698,18 @@
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
       <c r="T16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="8"/>
@@ -2721,28 +2721,28 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
       <c r="P17" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
       <c r="T17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="8"/>
@@ -2754,28 +2754,28 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
       <c r="T18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
@@ -2787,28 +2787,28 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
       <c r="P19" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
       <c r="T19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="8"/>
@@ -2820,28 +2820,28 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
       <c r="P20" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
       <c r="T20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="8"/>
@@ -2853,28 +2853,28 @@
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
       <c r="P21" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
       <c r="T21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="8"/>
@@ -2886,30 +2886,30 @@
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
       <c r="T22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
@@ -2921,30 +2921,30 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
       <c r="T23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="8"/>
@@ -2956,30 +2956,30 @@
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="N24" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="N24" s="8" t="s">
+      <c r="O24" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="O24" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
       <c r="T24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
@@ -2991,7 +2991,7 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
@@ -2999,18 +2999,18 @@
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
       <c r="T25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="8"/>
@@ -3022,28 +3022,28 @@
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N26" s="8"/>
       <c r="O26" s="8"/>
       <c r="P26" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
       <c r="T26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
@@ -3055,7 +3055,7 @@
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N27" s="8"/>
       <c r="O27" s="8"/>
@@ -3063,18 +3063,18 @@
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
       <c r="T27" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="8"/>
@@ -3086,30 +3086,30 @@
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P28" s="8"/>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
       <c r="T28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="8"/>
@@ -3121,30 +3121,30 @@
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
       <c r="M29" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="N29" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="O29" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="N29" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="O29" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
       <c r="T29" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="8"/>
@@ -3156,30 +3156,30 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
       <c r="M30" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
       <c r="T30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="8"/>
@@ -3191,7 +3191,7 @@
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
       <c r="M31" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>
@@ -3199,18 +3199,18 @@
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="T31" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="8"/>
@@ -3222,30 +3222,30 @@
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N32" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O32" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="N32" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="O32" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="P32" s="8"/>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="T32" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
@@ -3257,28 +3257,28 @@
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
       <c r="P33" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="T33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
@@ -3290,7 +3290,7 @@
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
@@ -3298,18 +3298,18 @@
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
       <c r="T34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="8"/>
@@ -3321,7 +3321,7 @@
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
@@ -3329,18 +3329,18 @@
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="T35" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="8"/>
@@ -3352,7 +3352,7 @@
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
       <c r="M36" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
@@ -3360,18 +3360,18 @@
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
       <c r="T36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="8"/>
@@ -3383,28 +3383,28 @@
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
       <c r="M37" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N37" s="8"/>
       <c r="O37" s="8"/>
       <c r="P37" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
       <c r="T37" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="8"/>
@@ -3416,30 +3416,30 @@
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="M38" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O38" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P38" s="8"/>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
       <c r="T38" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
@@ -3451,7 +3451,7 @@
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
       <c r="M39" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N39" s="8"/>
       <c r="O39" s="8"/>
@@ -3459,18 +3459,18 @@
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
       <c r="T39" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
@@ -3482,7 +3482,7 @@
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
       <c r="M40" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N40" s="8"/>
       <c r="O40" s="8"/>
@@ -3490,18 +3490,18 @@
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
       <c r="T40" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
@@ -3513,28 +3513,28 @@
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
       <c r="M41" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N41" s="8"/>
       <c r="O41" s="8"/>
       <c r="P41" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
       <c r="T41" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="8"/>
@@ -3546,7 +3546,7 @@
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
       <c r="M42" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N42" s="8"/>
       <c r="O42" s="8"/>
@@ -3554,18 +3554,18 @@
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
       <c r="T42" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="8"/>
@@ -3577,7 +3577,7 @@
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
       <c r="M43" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N43" s="8"/>
       <c r="O43" s="8"/>
@@ -3585,18 +3585,18 @@
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
       <c r="T43" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="8"/>
@@ -3608,28 +3608,28 @@
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
       <c r="M44" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N44" s="8"/>
       <c r="O44" s="8"/>
       <c r="P44" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
       <c r="T44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
@@ -3641,28 +3641,28 @@
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
       <c r="M45" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N45" s="8"/>
       <c r="O45" s="8"/>
       <c r="P45" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q45" s="8"/>
       <c r="R45" s="8"/>
       <c r="T45" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="8"/>
@@ -3674,28 +3674,28 @@
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="M46" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N46" s="8"/>
       <c r="O46" s="8"/>
       <c r="P46" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q46" s="8"/>
       <c r="R46" s="8"/>
       <c r="T46" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
@@ -3707,7 +3707,7 @@
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
       <c r="M47" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N47" s="8"/>
       <c r="O47" s="8"/>
@@ -3715,18 +3715,18 @@
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
       <c r="T47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="8"/>
@@ -3738,28 +3738,28 @@
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
       <c r="M48" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N48" s="8"/>
       <c r="O48" s="8"/>
       <c r="P48" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q48" s="8"/>
       <c r="R48" s="8"/>
       <c r="T48" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="8"/>
@@ -3771,28 +3771,28 @@
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
       <c r="M49" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N49" s="8"/>
       <c r="O49" s="8"/>
       <c r="P49" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q49" s="8"/>
       <c r="R49" s="8"/>
       <c r="T49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="8"/>
@@ -3804,28 +3804,28 @@
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
       <c r="M50" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N50" s="8"/>
       <c r="O50" s="8"/>
       <c r="P50" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q50" s="8"/>
       <c r="R50" s="8"/>
       <c r="T50" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
@@ -3837,28 +3837,28 @@
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
       <c r="M51" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N51" s="8"/>
       <c r="O51" s="8"/>
       <c r="P51" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q51" s="8"/>
       <c r="R51" s="8"/>
       <c r="T51" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="8"/>
@@ -3870,32 +3870,32 @@
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
       <c r="M52" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="N52" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="O52" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P52" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="N52" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="O52" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P52" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="Q52" s="8"/>
       <c r="R52" s="8"/>
       <c r="T52" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="8"/>
@@ -3907,7 +3907,7 @@
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
       <c r="M53" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N53" s="8"/>
       <c r="O53" s="8"/>
@@ -3915,18 +3915,18 @@
       <c r="Q53" s="8"/>
       <c r="R53" s="8"/>
       <c r="T53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="8"/>
@@ -3938,28 +3938,28 @@
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
       <c r="M54" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N54" s="8"/>
       <c r="O54" s="8"/>
       <c r="P54" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q54" s="8"/>
       <c r="R54" s="8"/>
       <c r="T54" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="8"/>
@@ -3971,7 +3971,7 @@
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
       <c r="M55" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N55" s="8"/>
       <c r="O55" s="8"/>
@@ -3979,18 +3979,18 @@
       <c r="Q55" s="8"/>
       <c r="R55" s="8"/>
       <c r="T55" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="8"/>
@@ -4002,28 +4002,28 @@
       <c r="K56" s="8"/>
       <c r="L56" s="8"/>
       <c r="M56" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N56" s="8"/>
       <c r="O56" s="8"/>
       <c r="P56" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Q56" s="8"/>
       <c r="R56" s="8"/>
       <c r="T56" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
@@ -4035,30 +4035,30 @@
       <c r="K57" s="8"/>
       <c r="L57" s="8"/>
       <c r="M57" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="N57" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="N57" s="8" t="s">
-        <v>149</v>
-      </c>
       <c r="O57" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P57" s="8"/>
       <c r="Q57" s="8"/>
       <c r="R57" s="8"/>
       <c r="T57" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="58" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="8"/>
@@ -4070,32 +4070,32 @@
       <c r="K58" s="8"/>
       <c r="L58" s="8"/>
       <c r="M58" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="N58" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O58" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P58" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="N58" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="O58" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="P58" s="8" t="s">
-        <v>152</v>
       </c>
       <c r="Q58" s="8"/>
       <c r="R58" s="8"/>
       <c r="T58" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="59" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="8"/>
@@ -4107,28 +4107,28 @@
       <c r="K59" s="8"/>
       <c r="L59" s="8"/>
       <c r="M59" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N59" s="8"/>
       <c r="O59" s="8"/>
       <c r="P59" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q59" s="8"/>
       <c r="R59" s="8"/>
       <c r="T59" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="60" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="8"/>
@@ -4140,28 +4140,28 @@
       <c r="K60" s="8"/>
       <c r="L60" s="8"/>
       <c r="M60" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N60" s="8"/>
       <c r="O60" s="8"/>
       <c r="P60" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q60" s="8"/>
       <c r="R60" s="8"/>
       <c r="T60" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="61" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="8"/>
@@ -4173,7 +4173,7 @@
       <c r="K61" s="8"/>
       <c r="L61" s="8"/>
       <c r="M61" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N61" s="8"/>
       <c r="O61" s="8"/>
@@ -4181,18 +4181,18 @@
       <c r="Q61" s="8"/>
       <c r="R61" s="8"/>
       <c r="T61" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="8"/>
@@ -4204,7 +4204,7 @@
       <c r="K62" s="8"/>
       <c r="L62" s="8"/>
       <c r="M62" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N62" s="8"/>
       <c r="O62" s="8"/>
@@ -4212,18 +4212,18 @@
       <c r="Q62" s="8"/>
       <c r="R62" s="8"/>
       <c r="T62" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
@@ -4235,30 +4235,30 @@
       <c r="K63" s="8"/>
       <c r="L63" s="8"/>
       <c r="M63" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N63" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O63" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P63" s="8"/>
       <c r="Q63" s="8"/>
       <c r="R63" s="8"/>
       <c r="T63" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D64" s="9"/>
       <c r="E64" s="8"/>
@@ -4270,30 +4270,30 @@
       <c r="K64" s="8"/>
       <c r="L64" s="8"/>
       <c r="M64" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N64" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O64" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P64" s="8"/>
       <c r="Q64" s="8"/>
       <c r="R64" s="8"/>
       <c r="T64" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D65" s="9"/>
       <c r="E65" s="8"/>
@@ -4305,30 +4305,30 @@
       <c r="K65" s="8"/>
       <c r="L65" s="8"/>
       <c r="M65" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N65" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O65" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P65" s="8"/>
       <c r="Q65" s="8"/>
       <c r="R65" s="8"/>
       <c r="T65" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="66" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="8"/>
@@ -4340,7 +4340,7 @@
       <c r="K66" s="8"/>
       <c r="L66" s="8"/>
       <c r="M66" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N66" s="8"/>
       <c r="O66" s="8"/>
@@ -4348,18 +4348,18 @@
       <c r="Q66" s="8"/>
       <c r="R66" s="8"/>
       <c r="T66" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="8"/>
@@ -4371,30 +4371,30 @@
       <c r="K67" s="8"/>
       <c r="L67" s="8"/>
       <c r="M67" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N67" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O67" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P67" s="8"/>
       <c r="Q67" s="8"/>
       <c r="R67" s="8"/>
       <c r="T67" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D68" s="9"/>
       <c r="E68" s="8"/>
@@ -4406,30 +4406,30 @@
       <c r="K68" s="8"/>
       <c r="L68" s="8"/>
       <c r="M68" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N68" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O68" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P68" s="8"/>
       <c r="Q68" s="8"/>
       <c r="R68" s="8"/>
       <c r="T68" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D69" s="9"/>
       <c r="E69" s="8"/>
@@ -4441,7 +4441,7 @@
       <c r="K69" s="8"/>
       <c r="L69" s="8"/>
       <c r="M69" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N69" s="8"/>
       <c r="O69" s="8"/>
@@ -4449,18 +4449,18 @@
       <c r="Q69" s="8"/>
       <c r="R69" s="8"/>
       <c r="T69" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D70" s="9"/>
       <c r="E70" s="8"/>
@@ -4472,7 +4472,7 @@
       <c r="K70" s="8"/>
       <c r="L70" s="8"/>
       <c r="M70" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N70" s="8"/>
       <c r="O70" s="8"/>
@@ -4480,18 +4480,18 @@
       <c r="Q70" s="8"/>
       <c r="R70" s="8"/>
       <c r="T70" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D71" s="9"/>
       <c r="E71" s="8"/>
@@ -4503,7 +4503,7 @@
       <c r="K71" s="8"/>
       <c r="L71" s="8"/>
       <c r="M71" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N71" s="8"/>
       <c r="O71" s="8"/>
@@ -4511,7 +4511,7 @@
       <c r="Q71" s="8"/>
       <c r="R71" s="8"/>
       <c r="T71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.2">
@@ -4758,18 +4758,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4792,18 +4792,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF9454A1-A395-40F6-B8A5-B468B9176A79}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F469C38F-E02B-4811-BC50-AB2CCD2039A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF9454A1-A395-40F6-B8A5-B468B9176A79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>